<commit_message>
random updates to sync
</commit_message>
<xml_diff>
--- a/analyses/Summary of Nonleafout and Leafouts.xlsx
+++ b/analyses/Summary of Nonleafout and Leafouts.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28040" windowHeight="26080" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Leafouts" sheetId="2" r:id="rId1"/>
-    <sheet name="Nonleafouts" sheetId="1" r:id="rId2"/>
+    <sheet name="Leafouts Rand" sheetId="3" r:id="rId1"/>
+    <sheet name="Leafouts" sheetId="2" r:id="rId2"/>
+    <sheet name="Nonleafouts" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="65">
   <si>
     <t>ACEPEN</t>
   </si>
@@ -670,7 +671,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1225,6 +1226,568 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M30"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" style="1"/>
+    <col min="2" max="5" width="11.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="2" customWidth="1"/>
+    <col min="8" max="9" width="11.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" style="2" customWidth="1"/>
+    <col min="11" max="12" width="11.83203125" style="1"/>
+    <col min="13" max="13" width="19.83203125" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="11.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="36">
+      <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="54">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" ht="36">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="36">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" ht="54">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" ht="54">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" ht="54">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" ht="54">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" ht="72">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" ht="72">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" ht="54">
+      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="K30" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>

</xml_diff>